<commit_message>
Update diagnostics results 5th May
</commit_message>
<xml_diff>
--- a/diagnostics/PES-Data Entry Performance.xlsx
+++ b/diagnostics/PES-Data Entry Performance.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="2017-05-02" r:id="rId3" sheetId="1"/>
+    <sheet name="2017-05-04" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="51">
   <si>
     <t>CreatedBy</t>
   </si>
@@ -138,6 +139,33 @@
   </si>
   <si>
     <t>Pui Yee</t>
+  </si>
+  <si>
+    <t>Default Administrator</t>
+  </si>
+  <si>
+    <t>Syahirah</t>
+  </si>
+  <si>
+    <t>DR ANG</t>
+  </si>
+  <si>
+    <t>Dr Saravanan</t>
+  </si>
+  <si>
+    <t>Adlan</t>
+  </si>
+  <si>
+    <t>Dr saravanan</t>
+  </si>
+  <si>
+    <t>Helmi</t>
+  </si>
+  <si>
+    <t>Jennifer Kaur</t>
+  </si>
+  <si>
+    <t>Natrah</t>
   </si>
 </sst>
 </file>
@@ -751,4 +779,703 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="n">
+        <v>443.0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>457.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>